<commit_message>
Actual budget type 2016
</commit_message>
<xml_diff>
--- a/data/uganda_data.xlsx
+++ b/data/uganda_data.xlsx
@@ -1741,6 +1741,894 @@
         <v>115</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="n">
+        <v>4.228113576</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="n">
+        <v>6.200835133</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.928820803</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>8.111995421</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4.915350471</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="n">
+        <v>4.311356158</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="n">
+        <v>9.456164157</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="n">
+        <v>4.05358077</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="n">
+        <v>4.132818882</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2.071230839</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2.857737724</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="n">
+        <v>17.22229157</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="n">
+        <v>7.014520702</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="n">
+        <v>4.09374665</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="n">
+        <v>7.786478257</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="n">
+        <v>15.08825748</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1.034532909</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1.110027373</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="n">
+        <v>4.320543264</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="n">
+        <v>3.729655082</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3.525435707</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3.481990246</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="n">
+        <v>3.266431571</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1.927994505</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="n">
+        <v>6.778855822</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2.462745987</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" t="n">
+        <v>16.42355031</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" t="n">
+        <v>3.517376768</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1.608049465</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" t="n">
+        <v>4.980181071</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1.392029936</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="n">
+        <v>9.595019052</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2.610555488</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2.975536557</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="n">
+        <v>6.809822205</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2.75053103</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2.467069511</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" t="n">
+        <v>3.793723202</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2.849326571</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1.738795025</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2.140894365</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" t="n">
+        <v>3.517518962</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1.076577002</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" t="n">
+        <v>1.794543918</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1.649481326</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" t="n">
+        <v>2.02271433</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1.928210664</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1.432557277</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1.980081092</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.876832771</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" t="n">
+        <v>2.735449271</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" t="n">
+        <v>17.30515742</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" t="n">
+        <v>3.322605908</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" t="n">
+        <v>3.632831354</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" t="n">
+        <v>3.776152656</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1.673787688</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1.318383842</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" t="n">
+        <v>4.130716814</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" t="n">
+        <v>9.021628928</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" t="n">
+        <v>4.675965757</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" t="n">
+        <v>1.577500045</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" t="n">
+        <v>3.628548853</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64" t="n">
+        <v>10.67343139</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" t="n">
+        <v>3.559383054</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" t="n">
+        <v>5.874964298</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>71</v>
+      </c>
+      <c r="B67" t="n">
+        <v>2.613852869</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" t="n">
+        <v>3.227068861</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69" t="n">
+        <v>1.651018678</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70" t="n">
+        <v>2.347885723</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>75</v>
+      </c>
+      <c r="B71" t="n">
+        <v>2.822657327</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" t="n">
+        <v>2.484235045</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0.678701506</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>78</v>
+      </c>
+      <c r="B74" t="n">
+        <v>1.520373983</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75" t="n">
+        <v>7.574696897</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76" t="n">
+        <v>1.149082006</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77" t="n">
+        <v>3.750093118</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>82</v>
+      </c>
+      <c r="B78" t="n">
+        <v>1.492727988</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>83</v>
+      </c>
+      <c r="B79" t="n">
+        <v>3.706730823</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80" t="n">
+        <v>1.85760389</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81" t="n">
+        <v>2.384976577</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>86</v>
+      </c>
+      <c r="B82" t="n">
+        <v>1.440055214</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>87</v>
+      </c>
+      <c r="B83" t="n">
+        <v>1.848119023</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>88</v>
+      </c>
+      <c r="B84" t="n">
+        <v>5.576876462</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>89</v>
+      </c>
+      <c r="B85" t="n">
+        <v>0.990125623</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>90</v>
+      </c>
+      <c r="B86" t="n">
+        <v>4.732565515</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0.876092318</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>92</v>
+      </c>
+      <c r="B88" t="n">
+        <v>4.793683145</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" t="n">
+        <v>8.455456865</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90" t="n">
+        <v>7.576963737</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" t="n">
+        <v>7.8994788</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92" t="n">
+        <v>7.357706527</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" t="n">
+        <v>4.221122879</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>97</v>
+      </c>
+      <c r="B94" t="n">
+        <v>3.71846899</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>98</v>
+      </c>
+      <c r="B95" t="n">
+        <v>7.666362083</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>9</v>
+      </c>
+      <c r="B96" t="n">
+        <v>9.791104918</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>99</v>
+      </c>
+      <c r="B97" t="n">
+        <v>4.986543693</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98" t="n">
+        <v>3.377879017</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>101</v>
+      </c>
+      <c r="B99" t="n">
+        <v>2.691414539</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100" t="n">
+        <v>2.762389883</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" t="n">
+        <v>5.045075423</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>104</v>
+      </c>
+      <c r="B102" t="n">
+        <v>4.884211801</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>105</v>
+      </c>
+      <c r="B103" t="n">
+        <v>4.511951216</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>106</v>
+      </c>
+      <c r="B104" t="n">
+        <v>3.88984054</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>107</v>
+      </c>
+      <c r="B105" t="n">
+        <v>4.953564944</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>108</v>
+      </c>
+      <c r="B106" t="n">
+        <v>2.312739042</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>109</v>
+      </c>
+      <c r="B107" t="n">
+        <v>5.953964849</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>110</v>
+      </c>
+      <c r="B108" t="n">
+        <v>5.320259901</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>111</v>
+      </c>
+      <c r="B109" t="n">
+        <v>2.367790319</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" t="n">
+        <v>3.470033105</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" t="n">
+        <v>2.556437304</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>114</v>
+      </c>
+      <c r="B112" t="n">
+        <v>2.147282692</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1763,6 +2651,874 @@
         <v>116</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="n">
+        <v>38.17819434</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.38602919</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.5223938</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4.566962476</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2.534015696</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="n">
+        <v>4.358035557</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.646161968</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2.928461183</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.479425872</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3.091866801</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.65331205</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2.495154615</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.803067859</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2.300000673</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="n">
+        <v>5.576662782</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.159278647</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="n">
+        <v>9.296888781</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2.142099403</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3.103697244</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2.617196036</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="n">
+        <v>3.432780699</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.202187044</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2.141113051</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1.577063883</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.030829113</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1.408626008</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" t="n">
+        <v>7.81758972</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" t="n">
+        <v>3.520069099</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="n">
+        <v>2.419111192</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="n">
+        <v>1.883406477</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0.563753712</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1.229870838</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="n">
+        <v>3.382151699</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" t="n">
+        <v>4.334403287</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2.603885364</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.065721209</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1.457515543</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2.640463722</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2.869007744</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="n">
+        <v>3.27979297</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" t="n">
+        <v>2.115468512</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" t="n">
+        <v>4.253905226</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" t="n">
+        <v>1.691753096</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" t="n">
+        <v>2.045734377</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1.057583525</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" t="n">
+        <v>7.102184186</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1.37779521</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0.912889569</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" t="n">
+        <v>10.96631953</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" t="n">
+        <v>9.938296818</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.648424056</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" t="n">
+        <v>3.073305866</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" t="n">
+        <v>3.985654224</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" t="n">
+        <v>7.562331028</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" t="n">
+        <v>1.655348691</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" t="n">
+        <v>2.950981474</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1.527187805</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>71</v>
+      </c>
+      <c r="B67" t="n">
+        <v>10.51478403</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" t="n">
+        <v>3.938739681</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69" t="n">
+        <v>9.943570708</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70" t="n">
+        <v>15.94206339</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>75</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1.474987818</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" t="n">
+        <v>5.468586952</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" t="n">
+        <v>4.085344994</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>78</v>
+      </c>
+      <c r="B74" t="n">
+        <v>6.689520165</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75" t="n">
+        <v>4.555951877</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76" t="n">
+        <v>5.393048514</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77" t="n">
+        <v>3.032703878</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>82</v>
+      </c>
+      <c r="B78" t="n">
+        <v>2.454301232</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>83</v>
+      </c>
+      <c r="B79" t="n">
+        <v>1.997174495</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80" t="n">
+        <v>6.96792064</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0.11500782</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>86</v>
+      </c>
+      <c r="B82" t="n">
+        <v>5.265889176</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>87</v>
+      </c>
+      <c r="B83" t="n">
+        <v>4.860103146</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>88</v>
+      </c>
+      <c r="B84"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>89</v>
+      </c>
+      <c r="B85" t="n">
+        <v>4.098517151</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>90</v>
+      </c>
+      <c r="B86" t="n">
+        <v>5.005857661</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87" t="n">
+        <v>2.690890239</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>92</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0.363249229</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.654599749</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90" t="n">
+        <v>1.359278289</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" t="n">
+        <v>1.600830967</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92" t="n">
+        <v>1.465678143</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" t="n">
+        <v>1.644487678</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>97</v>
+      </c>
+      <c r="B94" t="n">
+        <v>3.581977002</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>98</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0.824085556</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>9</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0.240180388</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>99</v>
+      </c>
+      <c r="B97" t="n">
+        <v>1.687900821</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>101</v>
+      </c>
+      <c r="B99" t="n">
+        <v>2.620469746</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100" t="n">
+        <v>3.336437983</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" t="n">
+        <v>5.02134159</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>104</v>
+      </c>
+      <c r="B102" t="n">
+        <v>1.998034567</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>105</v>
+      </c>
+      <c r="B103" t="n">
+        <v>4.179304355</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>106</v>
+      </c>
+      <c r="B104" t="n">
+        <v>0.248657145</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>107</v>
+      </c>
+      <c r="B105" t="n">
+        <v>4.660560717</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>108</v>
+      </c>
+      <c r="B106" t="n">
+        <v>1.313051236</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>109</v>
+      </c>
+      <c r="B107" t="n">
+        <v>1.411956431</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>110</v>
+      </c>
+      <c r="B108" t="n">
+        <v>6.805162763</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>111</v>
+      </c>
+      <c r="B109" t="n">
+        <v>0.483606672</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" t="n">
+        <v>7.479174133</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" t="n">
+        <v>1.508198871</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>114</v>
+      </c>
+      <c r="B112" t="n">
+        <v>0.883457294</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Update to 2017 actual
</commit_message>
<xml_diff>
--- a/data/uganda_data.xlsx
+++ b/data/uganda_data.xlsx
@@ -1746,7 +1746,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="n">
-        <v>4.228113576</v>
+        <v>4.541639438</v>
       </c>
     </row>
     <row r="3">
@@ -1754,7 +1754,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="n">
-        <v>6.200835133</v>
+        <v>5.203772724</v>
       </c>
     </row>
     <row r="4">
@@ -1762,7 +1762,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="n">
-        <v>0.928820803</v>
+        <v>0.916304667</v>
       </c>
     </row>
     <row r="5">
@@ -1770,7 +1770,7 @@
         <v>18</v>
       </c>
       <c r="B5" t="n">
-        <v>8.111995421</v>
+        <v>14.18571894</v>
       </c>
     </row>
     <row r="6">
@@ -1778,7 +1778,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="n">
-        <v>4.915350471</v>
+        <v>4.139156418</v>
       </c>
     </row>
     <row r="7">
@@ -1786,7 +1786,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="n">
-        <v>4.311356158</v>
+        <v>3.538695403</v>
       </c>
     </row>
     <row r="8">
@@ -1794,839 +1794,599 @@
         <v>21</v>
       </c>
       <c r="B8" t="n">
-        <v>9.456164157</v>
+        <v>4.088950403</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" t="n">
-        <v>4.05358077</v>
+        <v>4.085117158</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" t="n">
-        <v>4.132818882</v>
+        <v>4.052338098</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>2.071230839</v>
+        <v>16.87423146</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" t="n">
-        <v>2.857737724</v>
+        <v>5.983323335</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B13" t="n">
-        <v>17.22229157</v>
+        <v>4.756896631</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B14" t="n">
-        <v>7.014520702</v>
+        <v>28.25647561</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B15" t="n">
-        <v>4.09374665</v>
+        <v>0.732599047</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B16" t="n">
-        <v>7.786478257</v>
+        <v>4.0636447</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B17" t="n">
-        <v>15.08825748</v>
+        <v>3.901773227</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B18" t="n">
-        <v>1.034532909</v>
+        <v>3.486128824</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B19" t="n">
-        <v>1.110027373</v>
+        <v>3.861227727</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B20" t="n">
-        <v>4.320543264</v>
+        <v>0.978339196</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B21" t="n">
-        <v>3.729655082</v>
+        <v>38.83940352</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B22" t="n">
-        <v>3.525435707</v>
+        <v>2.787675764</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B23" t="n">
-        <v>3.481990246</v>
+        <v>2.72585879</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B24" t="n">
-        <v>3.266431571</v>
+        <v>12.91936959</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B25" t="n">
-        <v>1.927994505</v>
+        <v>1.692963805</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B26" t="n">
-        <v>6.778855822</v>
+        <v>6.241647428</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B27" t="n">
-        <v>2.462745987</v>
+        <v>6.474493141</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B28" t="n">
-        <v>16.42355031</v>
+        <v>1.946048319</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B29" t="n">
-        <v>3.517376768</v>
+        <v>1.813154734</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B30" t="n">
-        <v>1.608049465</v>
+        <v>2.560169377</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B31" t="n">
-        <v>4.980181071</v>
+        <v>1.298996415</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B32" t="n">
-        <v>1.392029936</v>
+        <v>1.798340469</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="B33" t="n">
-        <v>9.595019052</v>
+        <v>0.978339196</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B34" t="n">
-        <v>2.610555488</v>
+        <v>2.329644826</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B35" t="n">
-        <v>2.975536557</v>
+        <v>2.297467716</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="B36" t="n">
-        <v>6.809822205</v>
+        <v>1.674426788</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B37" t="n">
-        <v>2.75053103</v>
+        <v>0.46408253</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B38" t="n">
-        <v>2.467069511</v>
+        <v>1.785610351</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B39" t="n">
-        <v>3.793723202</v>
+        <v>0.489512484</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="B40" t="n">
-        <v>2.849326571</v>
+        <v>4.441923821</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="B41" t="n">
-        <v>1.738795025</v>
+        <v>4.405825572</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B42" t="n">
-        <v>2.140894365</v>
+        <v>1.134584252</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="B43" t="n">
-        <v>3.517518962</v>
+        <v>4.276503322</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="B44" t="n">
-        <v>1.076577002</v>
+        <v>2.264433981</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B45" t="n">
-        <v>1.794543918</v>
+        <v>2.242613489</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="B46" t="n">
-        <v>1.649481326</v>
+        <v>4.014831409</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="B47" t="n">
-        <v>2.02271433</v>
+        <v>2.998551509</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B48" t="n">
-        <v>1.928210664</v>
+        <v>9.326400989</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B49" t="n">
-        <v>1.432557277</v>
+        <v>1.400130352</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B50" t="n">
-        <v>1.980081092</v>
+        <v>1.806781911</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B51" t="n">
-        <v>0.876832771</v>
+        <v>2.198432456</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B52" t="n">
-        <v>2.735449271</v>
+        <v>2.424495698</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B53" t="n">
-        <v>17.30515742</v>
+        <v>0.817709415</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B54" t="n">
-        <v>3.322605908</v>
+        <v>4.184856282</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B55" t="n">
-        <v>3.632831354</v>
+        <v>1.216133273</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B56" t="n">
-        <v>3.776152656</v>
+        <v>2.063990747</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="B57" t="n">
-        <v>1.673787688</v>
+        <v>2.069804033</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="B58" t="n">
-        <v>1.318383842</v>
+        <v>2.069099584</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="B59" t="n">
-        <v>4.130716814</v>
+        <v>1.74498138</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="B60" t="n">
-        <v>9.021628928</v>
+        <v>7.419495079</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="B61" t="n">
-        <v>4.675965757</v>
+        <v>12.34923114</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="B62" t="n">
-        <v>1.577500045</v>
+        <v>6.558630433</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="B63" t="n">
-        <v>3.628548853</v>
+        <v>8.995898879</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="B64" t="n">
-        <v>10.67343139</v>
+        <v>8.373917445</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="B65" t="n">
-        <v>3.559383054</v>
+        <v>12.83532329</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="B66" t="n">
-        <v>5.874964298</v>
+        <v>3.103542477</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="B67" t="n">
-        <v>2.613852869</v>
+        <v>27.85784585</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="B68" t="n">
-        <v>3.227068861</v>
+        <v>16.21956159</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="B69" t="n">
-        <v>1.651018678</v>
+        <v>13.83125798</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="B70" t="n">
-        <v>2.347885723</v>
+        <v>4.439137549</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="B71" t="n">
-        <v>2.822657327</v>
+        <v>1.799115782</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="B72" t="n">
-        <v>2.484235045</v>
+        <v>2.611909214</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="B73" t="n">
-        <v>0.678701506</v>
+        <v>2.078787564</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="B74" t="n">
-        <v>1.520373983</v>
+        <v>3.556581677</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B75" t="n">
-        <v>7.574696897</v>
+        <v>7.25330341</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="B76" t="n">
-        <v>1.149082006</v>
+        <v>3.898251801</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="B77" t="n">
-        <v>3.750093118</v>
+        <v>6.671384551</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="B78" t="n">
-        <v>1.492727988</v>
+        <v>5.594435146</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="B79" t="n">
-        <v>3.706730823</v>
+        <v>1.547664591</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="B80" t="n">
-        <v>1.85760389</v>
+        <v>1.728132866</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="B81" t="n">
-        <v>2.384976577</v>
+        <v>2.853950334</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="B82" t="n">
-        <v>1.440055214</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s">
-        <v>87</v>
-      </c>
-      <c r="B83" t="n">
-        <v>1.848119023</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84" t="n">
-        <v>5.576876462</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>89</v>
-      </c>
-      <c r="B85" t="n">
-        <v>0.990125623</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s">
-        <v>90</v>
-      </c>
-      <c r="B86" t="n">
-        <v>4.732565515</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s">
-        <v>91</v>
-      </c>
-      <c r="B87" t="n">
-        <v>0.876092318</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s">
-        <v>92</v>
-      </c>
-      <c r="B88" t="n">
-        <v>4.793683145</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s">
-        <v>93</v>
-      </c>
-      <c r="B89" t="n">
-        <v>8.455456865</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s">
-        <v>94</v>
-      </c>
-      <c r="B90" t="n">
-        <v>7.576963737</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s">
-        <v>5</v>
-      </c>
-      <c r="B91" t="n">
-        <v>7.8994788</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="s">
-        <v>95</v>
-      </c>
-      <c r="B92" t="n">
-        <v>7.357706527</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s">
-        <v>96</v>
-      </c>
-      <c r="B93" t="n">
-        <v>4.221122879</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s">
-        <v>97</v>
-      </c>
-      <c r="B94" t="n">
-        <v>3.71846899</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s">
-        <v>98</v>
-      </c>
-      <c r="B95" t="n">
-        <v>7.666362083</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s">
-        <v>9</v>
-      </c>
-      <c r="B96" t="n">
-        <v>9.791104918</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s">
-        <v>99</v>
-      </c>
-      <c r="B97" t="n">
-        <v>4.986543693</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s">
-        <v>100</v>
-      </c>
-      <c r="B98" t="n">
-        <v>3.377879017</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="s">
-        <v>101</v>
-      </c>
-      <c r="B99" t="n">
-        <v>2.691414539</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s">
-        <v>102</v>
-      </c>
-      <c r="B100" t="n">
-        <v>2.762389883</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="s">
-        <v>103</v>
-      </c>
-      <c r="B101" t="n">
-        <v>5.045075423</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="s">
-        <v>104</v>
-      </c>
-      <c r="B102" t="n">
-        <v>4.884211801</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s">
-        <v>105</v>
-      </c>
-      <c r="B103" t="n">
-        <v>4.511951216</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="s">
-        <v>106</v>
-      </c>
-      <c r="B104" t="n">
-        <v>3.88984054</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="s">
-        <v>107</v>
-      </c>
-      <c r="B105" t="n">
-        <v>4.953564944</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="s">
-        <v>108</v>
-      </c>
-      <c r="B106" t="n">
-        <v>2.312739042</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="s">
-        <v>109</v>
-      </c>
-      <c r="B107" t="n">
-        <v>5.953964849</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="s">
-        <v>110</v>
-      </c>
-      <c r="B108" t="n">
-        <v>5.320259901</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="s">
-        <v>111</v>
-      </c>
-      <c r="B109" t="n">
-        <v>2.367790319</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="s">
-        <v>112</v>
-      </c>
-      <c r="B110" t="n">
-        <v>3.470033105</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="s">
-        <v>113</v>
-      </c>
-      <c r="B111" t="n">
-        <v>2.556437304</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="s">
-        <v>114</v>
-      </c>
-      <c r="B112" t="n">
-        <v>2.147282692</v>
+        <v>1.942748259</v>
       </c>
     </row>
   </sheetData>
@@ -2656,7 +2416,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="n">
-        <v>38.17819434</v>
+        <v>53.31404308</v>
       </c>
     </row>
     <row r="3">
@@ -2664,7 +2424,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="n">
-        <v>0.38602919</v>
+        <v>1.408770599</v>
       </c>
     </row>
     <row r="4">
@@ -2672,23 +2432,21 @@
         <v>17</v>
       </c>
       <c r="B4" t="n">
-        <v>1.5223938</v>
+        <v>1.774007196</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="n">
-        <v>4.566962476</v>
-      </c>
+      <c r="B5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="n">
-        <v>2.534015696</v>
+        <v>10.09650351</v>
       </c>
     </row>
     <row r="7">
@@ -2696,827 +2454,583 @@
         <v>20</v>
       </c>
       <c r="B7" t="n">
-        <v>4.358035557</v>
+        <v>3.610177056</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" t="n">
+        <v>2.841294712</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" t="n">
-        <v>0.646161968</v>
+        <v>3.113850986</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" t="n">
-        <v>2.928461183</v>
+        <v>3.627060691</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>1.479425872</v>
+        <v>1.880065746</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" t="n">
-        <v>3.091866801</v>
+        <v>2.87234637</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B13" t="n">
-        <v>0.65331205</v>
+        <v>0.533288975</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="n">
-        <v>2.495154615</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0.803067859</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16"/>
+        <v>31</v>
+      </c>
+      <c r="B16" t="n">
+        <v>6.696821022</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B17" t="n">
-        <v>2.300000673</v>
+        <v>2.176079603</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B18" t="n">
-        <v>5.576662782</v>
+        <v>3.256363829</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B19" t="n">
-        <v>0.159278647</v>
+        <v>2.27902315</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B20" t="n">
-        <v>9.296888781</v>
+        <v>1.625933957</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="n">
-        <v>2.142099403</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B21"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B22" t="n">
-        <v>3.103697244</v>
+        <v>1.43976639</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23"/>
+        <v>40</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.496146093</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" t="n">
-        <v>2.617196036</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B25" t="n">
-        <v>3.432780699</v>
+        <v>5.820147339</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B26" t="n">
-        <v>0.202187044</v>
+        <v>3.243644532</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B27" t="n">
-        <v>2.141113051</v>
+        <v>1.438782402</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B28" t="n">
-        <v>1.577063883</v>
+        <v>14.38747837</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B29" t="n">
-        <v>0.030829113</v>
+        <v>1.89660106</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B30" t="n">
-        <v>1.408626008</v>
+        <v>1.86650182</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B31" t="n">
-        <v>7.81758972</v>
+        <v>0.546306064</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B32" t="n">
-        <v>3.520069099</v>
+        <v>3.125688367</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="B33" t="n">
-        <v>2.419111192</v>
+        <v>1.625933957</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B34" t="n">
-        <v>1.883406477</v>
+        <v>2.675016686</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B35" t="n">
-        <v>0.563753712</v>
+        <v>1.63010458</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="B36" t="n">
-        <v>1.229870838</v>
+        <v>1.163413673</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" t="n">
-        <v>3.382151699</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B37"/>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B38" t="n">
-        <v>4.334403287</v>
+        <v>1.182252391</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B39" t="n">
-        <v>2.603885364</v>
+        <v>6.527998504</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" t="n">
-        <v>0.065721209</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B40"/>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="B41" t="n">
-        <v>1.457515543</v>
+        <v>0.823012001</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B42" t="n">
-        <v>2.640463722</v>
+        <v>14.97864358</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="B43" t="n">
-        <v>2.869007744</v>
+        <v>1.555069352</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="B44" t="n">
-        <v>3.27979297</v>
+        <v>1.789579143</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B45" t="n">
-        <v>2.115468512</v>
+        <v>17.88763843</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="B46" t="n">
-        <v>4.253905226</v>
+        <v>1.580202818</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="B47" t="n">
-        <v>1.691753096</v>
+        <v>23.81550264</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" t="n">
-        <v>2.045734377</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B48"/>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>56</v>
-      </c>
-      <c r="B49"/>
+        <v>71</v>
+      </c>
+      <c r="B49" t="n">
+        <v>16.35479354</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B50" t="n">
-        <v>1.057583525</v>
+        <v>8.789180489</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>58</v>
-      </c>
-      <c r="B51"/>
+        <v>75</v>
+      </c>
+      <c r="B51" t="n">
+        <v>49.44722943</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>59</v>
-      </c>
-      <c r="B52"/>
+        <v>76</v>
+      </c>
+      <c r="B52" t="n">
+        <v>2.355256429</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>60</v>
-      </c>
-      <c r="B53"/>
+        <v>77</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1.812884594</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B54" t="n">
-        <v>7.102184186</v>
+        <v>13.72285981</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B55" t="n">
-        <v>1.37779521</v>
+        <v>2.320414688</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B56" t="n">
-        <v>0.912889569</v>
+        <v>12.9731581</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="B57" t="n">
-        <v>10.96631953</v>
+        <v>0.957801758</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="B58" t="n">
-        <v>9.938296818</v>
+        <v>8.242166581</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="B59" t="n">
-        <v>0.648424056</v>
+        <v>0.596423192</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="B60" t="n">
-        <v>3.073305866</v>
+        <v>3.011438326</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>66</v>
-      </c>
-      <c r="B61" t="n">
-        <v>3.985654224</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="B61"/>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="B62" t="n">
-        <v>7.562331028</v>
+        <v>3.440094174</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>7</v>
-      </c>
-      <c r="B63" t="n">
-        <v>1.655348691</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B63"/>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64"/>
+        <v>5</v>
+      </c>
+      <c r="B64" t="n">
+        <v>1.106719661</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="B65" t="n">
-        <v>2.950981474</v>
+        <v>1.883875474</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="B66" t="n">
-        <v>1.527187805</v>
+        <v>4.388483053</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>71</v>
-      </c>
-      <c r="B67" t="n">
-        <v>10.51478403</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="B67"/>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>72</v>
-      </c>
-      <c r="B68" t="n">
-        <v>3.938739681</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B68"/>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>73</v>
-      </c>
-      <c r="B69" t="n">
-        <v>9.943570708</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B69"/>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="B70" t="n">
-        <v>15.94206339</v>
+        <v>10.14051046</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="B71" t="n">
-        <v>1.474987818</v>
+        <v>0.882331804</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="B72" t="n">
-        <v>5.468586952</v>
+        <v>1.056106401</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="B73" t="n">
-        <v>4.085344994</v>
+        <v>4.949204454</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="B74" t="n">
-        <v>6.689520165</v>
+        <v>2.894125184</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B75" t="n">
-        <v>4.555951877</v>
+        <v>4.07684759</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="B76" t="n">
-        <v>5.393048514</v>
+        <v>2.644795613</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="B77" t="n">
-        <v>3.032703878</v>
+        <v>5.558078944</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="B78" t="n">
-        <v>2.454301232</v>
+        <v>0.794105668</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="B79" t="n">
-        <v>1.997174495</v>
+        <v>5.124140376</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="B80" t="n">
-        <v>6.96792064</v>
+        <v>0.230206164</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="B81" t="n">
-        <v>0.11500782</v>
+        <v>3.415749762</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="B82" t="n">
-        <v>5.265889176</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s">
-        <v>87</v>
-      </c>
-      <c r="B83" t="n">
-        <v>4.860103146</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84"/>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>89</v>
-      </c>
-      <c r="B85" t="n">
-        <v>4.098517151</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s">
-        <v>90</v>
-      </c>
-      <c r="B86" t="n">
-        <v>5.005857661</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s">
-        <v>91</v>
-      </c>
-      <c r="B87" t="n">
-        <v>2.690890239</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s">
-        <v>92</v>
-      </c>
-      <c r="B88" t="n">
-        <v>0.363249229</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s">
-        <v>93</v>
-      </c>
-      <c r="B89" t="n">
-        <v>0.654599749</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s">
-        <v>94</v>
-      </c>
-      <c r="B90" t="n">
-        <v>1.359278289</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s">
-        <v>5</v>
-      </c>
-      <c r="B91" t="n">
-        <v>1.600830967</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="s">
-        <v>95</v>
-      </c>
-      <c r="B92" t="n">
-        <v>1.465678143</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s">
-        <v>96</v>
-      </c>
-      <c r="B93" t="n">
-        <v>1.644487678</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s">
-        <v>97</v>
-      </c>
-      <c r="B94" t="n">
-        <v>3.581977002</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s">
-        <v>98</v>
-      </c>
-      <c r="B95" t="n">
-        <v>0.824085556</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s">
-        <v>9</v>
-      </c>
-      <c r="B96" t="n">
-        <v>0.240180388</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s">
-        <v>99</v>
-      </c>
-      <c r="B97" t="n">
-        <v>1.687900821</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s">
-        <v>100</v>
-      </c>
-      <c r="B98"/>
-    </row>
-    <row r="99">
-      <c r="A99" t="s">
-        <v>101</v>
-      </c>
-      <c r="B99" t="n">
-        <v>2.620469746</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s">
-        <v>102</v>
-      </c>
-      <c r="B100" t="n">
-        <v>3.336437983</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="s">
-        <v>103</v>
-      </c>
-      <c r="B101" t="n">
-        <v>5.02134159</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="s">
-        <v>104</v>
-      </c>
-      <c r="B102" t="n">
-        <v>1.998034567</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s">
-        <v>105</v>
-      </c>
-      <c r="B103" t="n">
-        <v>4.179304355</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="s">
-        <v>106</v>
-      </c>
-      <c r="B104" t="n">
-        <v>0.248657145</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="s">
-        <v>107</v>
-      </c>
-      <c r="B105" t="n">
-        <v>4.660560717</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="s">
-        <v>108</v>
-      </c>
-      <c r="B106" t="n">
-        <v>1.313051236</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="s">
-        <v>109</v>
-      </c>
-      <c r="B107" t="n">
-        <v>1.411956431</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="s">
-        <v>110</v>
-      </c>
-      <c r="B108" t="n">
-        <v>6.805162763</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="s">
-        <v>111</v>
-      </c>
-      <c r="B109" t="n">
-        <v>0.483606672</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="s">
-        <v>112</v>
-      </c>
-      <c r="B110" t="n">
-        <v>7.479174133</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="s">
-        <v>113</v>
-      </c>
-      <c r="B111" t="n">
-        <v>1.508198871</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="s">
-        <v>114</v>
-      </c>
-      <c r="B112" t="n">
-        <v>0.883457294</v>
+        <v>1.157516618</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pov 2014, local/donor 2016
</commit_message>
<xml_diff>
--- a/data/uganda_data.xlsx
+++ b/data/uganda_data.xlsx
@@ -1746,7 +1746,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="n">
-        <v>4.541639438</v>
+        <v>4.228113576</v>
       </c>
     </row>
     <row r="3">
@@ -1754,7 +1754,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="n">
-        <v>5.203772724</v>
+        <v>6.200835133</v>
       </c>
     </row>
     <row r="4">
@@ -1762,7 +1762,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="n">
-        <v>0.916304667</v>
+        <v>0.928820803</v>
       </c>
     </row>
     <row r="5">
@@ -1770,7 +1770,7 @@
         <v>18</v>
       </c>
       <c r="B5" t="n">
-        <v>14.18571894</v>
+        <v>8.111995421</v>
       </c>
     </row>
     <row r="6">
@@ -1778,7 +1778,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="n">
-        <v>4.139156418</v>
+        <v>4.915350471</v>
       </c>
     </row>
     <row r="7">
@@ -1786,7 +1786,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="n">
-        <v>3.538695403</v>
+        <v>4.311356158</v>
       </c>
     </row>
     <row r="8">
@@ -1794,599 +1794,839 @@
         <v>21</v>
       </c>
       <c r="B8" t="n">
-        <v>4.088950403</v>
+        <v>9.456164157</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" t="n">
-        <v>4.085117158</v>
+        <v>4.05358077</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" t="n">
-        <v>4.052338098</v>
+        <v>4.132818882</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B11" t="n">
-        <v>16.87423146</v>
+        <v>2.071230839</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="n">
-        <v>5.983323335</v>
+        <v>2.857737724</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B13" t="n">
-        <v>4.756896631</v>
+        <v>17.22229157</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" t="n">
-        <v>28.25647561</v>
+        <v>7.014520702</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B15" t="n">
-        <v>0.732599047</v>
+        <v>4.09374665</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B16" t="n">
-        <v>4.0636447</v>
+        <v>7.786478257</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B17" t="n">
-        <v>3.901773227</v>
+        <v>15.08825748</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B18" t="n">
-        <v>3.486128824</v>
+        <v>1.034532909</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B19" t="n">
-        <v>3.861227727</v>
+        <v>1.110027373</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B20" t="n">
-        <v>0.978339196</v>
+        <v>4.320543264</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B21" t="n">
-        <v>38.83940352</v>
+        <v>3.729655082</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B22" t="n">
-        <v>2.787675764</v>
+        <v>3.525435707</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B23" t="n">
-        <v>2.72585879</v>
+        <v>3.481990246</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B24" t="n">
-        <v>12.91936959</v>
+        <v>3.266431571</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B25" t="n">
-        <v>1.692963805</v>
+        <v>1.927994505</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B26" t="n">
-        <v>6.241647428</v>
+        <v>6.778855822</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B27" t="n">
-        <v>6.474493141</v>
+        <v>2.462745987</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="B28" t="n">
-        <v>1.946048319</v>
+        <v>16.42355031</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B29" t="n">
-        <v>1.813154734</v>
+        <v>3.517376768</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B30" t="n">
-        <v>2.560169377</v>
+        <v>1.608049465</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B31" t="n">
-        <v>1.298996415</v>
+        <v>4.980181071</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B32" t="n">
-        <v>1.798340469</v>
+        <v>1.392029936</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="B33" t="n">
-        <v>0.978339196</v>
+        <v>9.595019052</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B34" t="n">
-        <v>2.329644826</v>
+        <v>2.610555488</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="B35" t="n">
-        <v>2.297467716</v>
+        <v>2.975536557</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="B36" t="n">
-        <v>1.674426788</v>
+        <v>6.809822205</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B37" t="n">
-        <v>0.46408253</v>
+        <v>2.75053103</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B38" t="n">
-        <v>1.785610351</v>
+        <v>2.467069511</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B39" t="n">
-        <v>0.489512484</v>
+        <v>3.793723202</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B40" t="n">
-        <v>4.441923821</v>
+        <v>2.849326571</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B41" t="n">
-        <v>4.405825572</v>
+        <v>1.738795025</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B42" t="n">
-        <v>1.134584252</v>
+        <v>2.140894365</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="B43" t="n">
-        <v>4.276503322</v>
+        <v>3.517518962</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="B44" t="n">
-        <v>2.264433981</v>
+        <v>1.076577002</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B45" t="n">
-        <v>2.242613489</v>
+        <v>1.794543918</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B46" t="n">
-        <v>4.014831409</v>
+        <v>1.649481326</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B47" t="n">
-        <v>2.998551509</v>
+        <v>2.02271433</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B48" t="n">
-        <v>9.326400989</v>
+        <v>1.928210664</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B49" t="n">
-        <v>1.400130352</v>
+        <v>1.432557277</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B50" t="n">
-        <v>1.806781911</v>
+        <v>1.980081092</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B51" t="n">
-        <v>2.198432456</v>
+        <v>0.876832771</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="B52" t="n">
-        <v>2.424495698</v>
+        <v>2.735449271</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B53" t="n">
-        <v>0.817709415</v>
+        <v>17.30515742</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B54" t="n">
-        <v>4.184856282</v>
+        <v>3.322605908</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B55" t="n">
-        <v>1.216133273</v>
+        <v>3.632831354</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B56" t="n">
-        <v>2.063990747</v>
+        <v>3.776152656</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B57" t="n">
-        <v>2.069804033</v>
+        <v>1.673787688</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="B58" t="n">
-        <v>2.069099584</v>
+        <v>1.318383842</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="B59" t="n">
-        <v>1.74498138</v>
+        <v>4.130716814</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="B60" t="n">
-        <v>7.419495079</v>
+        <v>9.021628928</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="B61" t="n">
-        <v>12.34923114</v>
+        <v>4.675965757</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="B62" t="n">
-        <v>6.558630433</v>
+        <v>1.577500045</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="B63" t="n">
-        <v>8.995898879</v>
+        <v>3.628548853</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="B64" t="n">
-        <v>8.373917445</v>
+        <v>10.67343139</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="B65" t="n">
-        <v>12.83532329</v>
+        <v>3.559383054</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B66" t="n">
-        <v>3.103542477</v>
+        <v>5.874964298</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="B67" t="n">
-        <v>27.85784585</v>
+        <v>2.613852869</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="B68" t="n">
-        <v>16.21956159</v>
+        <v>3.227068861</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="B69" t="n">
-        <v>13.83125798</v>
+        <v>1.651018678</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="B70" t="n">
-        <v>4.439137549</v>
+        <v>2.347885723</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="B71" t="n">
-        <v>1.799115782</v>
+        <v>2.822657327</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="B72" t="n">
-        <v>2.611909214</v>
+        <v>2.484235045</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="B73" t="n">
-        <v>2.078787564</v>
+        <v>0.678701506</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="B74" t="n">
-        <v>3.556581677</v>
+        <v>1.520373983</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="B75" t="n">
-        <v>7.25330341</v>
+        <v>7.574696897</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="B76" t="n">
-        <v>3.898251801</v>
+        <v>1.149082006</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="B77" t="n">
-        <v>6.671384551</v>
+        <v>3.750093118</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="B78" t="n">
-        <v>5.594435146</v>
+        <v>1.492727988</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="B79" t="n">
-        <v>1.547664591</v>
+        <v>3.706730823</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="B80" t="n">
-        <v>1.728132866</v>
+        <v>1.85760389</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="B81" t="n">
-        <v>2.853950334</v>
+        <v>2.384976577</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
+        <v>86</v>
+      </c>
+      <c r="B82" t="n">
+        <v>1.440055214</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>87</v>
+      </c>
+      <c r="B83" t="n">
+        <v>1.848119023</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>88</v>
+      </c>
+      <c r="B84" t="n">
+        <v>5.576876462</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>89</v>
+      </c>
+      <c r="B85" t="n">
+        <v>0.990125623</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>90</v>
+      </c>
+      <c r="B86" t="n">
+        <v>4.732565515</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0.876092318</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>92</v>
+      </c>
+      <c r="B88" t="n">
+        <v>4.793683145</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" t="n">
+        <v>8.455456865</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90" t="n">
+        <v>7.576963737</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" t="n">
+        <v>7.8994788</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92" t="n">
+        <v>7.357706527</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" t="n">
+        <v>4.221122879</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>97</v>
+      </c>
+      <c r="B94" t="n">
+        <v>3.71846899</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>98</v>
+      </c>
+      <c r="B95" t="n">
+        <v>7.666362083</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>9</v>
+      </c>
+      <c r="B96" t="n">
+        <v>9.791104918</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>99</v>
+      </c>
+      <c r="B97" t="n">
+        <v>4.986543693</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98" t="n">
+        <v>3.377879017</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>101</v>
+      </c>
+      <c r="B99" t="n">
+        <v>2.691414539</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100" t="n">
+        <v>2.762389883</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" t="n">
+        <v>5.045075423</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>104</v>
+      </c>
+      <c r="B102" t="n">
+        <v>4.884211801</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>105</v>
+      </c>
+      <c r="B103" t="n">
+        <v>4.511951216</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>106</v>
+      </c>
+      <c r="B104" t="n">
+        <v>3.88984054</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>107</v>
+      </c>
+      <c r="B105" t="n">
+        <v>4.953564944</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>108</v>
+      </c>
+      <c r="B106" t="n">
+        <v>2.312739042</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>109</v>
+      </c>
+      <c r="B107" t="n">
+        <v>5.953964849</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>110</v>
+      </c>
+      <c r="B108" t="n">
+        <v>5.320259901</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>111</v>
+      </c>
+      <c r="B109" t="n">
+        <v>2.367790319</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" t="n">
+        <v>3.470033105</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" t="n">
+        <v>2.556437304</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
         <v>114</v>
       </c>
-      <c r="B82" t="n">
-        <v>1.942748259</v>
+      <c r="B112" t="n">
+        <v>2.147282692</v>
       </c>
     </row>
   </sheetData>
@@ -2416,7 +2656,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="n">
-        <v>53.31404308</v>
+        <v>38.17819434</v>
       </c>
     </row>
     <row r="3">
@@ -2424,7 +2664,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="n">
-        <v>1.408770599</v>
+        <v>0.38602919</v>
       </c>
     </row>
     <row r="4">
@@ -2432,21 +2672,23 @@
         <v>17</v>
       </c>
       <c r="B4" t="n">
-        <v>1.774007196</v>
+        <v>1.5223938</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" t="n">
+        <v>4.566962476</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="n">
-        <v>10.09650351</v>
+        <v>2.534015696</v>
       </c>
     </row>
     <row r="7">
@@ -2454,583 +2696,827 @@
         <v>20</v>
       </c>
       <c r="B7" t="n">
-        <v>3.610177056</v>
+        <v>4.358035557</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="n">
-        <v>2.841294712</v>
-      </c>
+      <c r="B8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" t="n">
-        <v>3.113850986</v>
+        <v>0.646161968</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" t="n">
-        <v>3.627060691</v>
+        <v>2.928461183</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B11" t="n">
-        <v>1.880065746</v>
+        <v>1.479425872</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="n">
-        <v>2.87234637</v>
+        <v>3.091866801</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B13" t="n">
-        <v>0.533288975</v>
+        <v>0.65331205</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14"/>
+        <v>26</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2.495154615</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15"/>
+        <v>10</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.803067859</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" t="n">
-        <v>6.696821022</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B17" t="n">
-        <v>2.176079603</v>
+        <v>2.300000673</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B18" t="n">
-        <v>3.256363829</v>
+        <v>5.576662782</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B19" t="n">
-        <v>2.27902315</v>
+        <v>0.159278647</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B20" t="n">
-        <v>1.625933957</v>
+        <v>9.296888781</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21"/>
+        <v>32</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2.142099403</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B22" t="n">
-        <v>1.43976639</v>
+        <v>3.103697244</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" t="n">
-        <v>0.496146093</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24"/>
+        <v>35</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2.617196036</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B25" t="n">
-        <v>5.820147339</v>
+        <v>3.432780699</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B26" t="n">
-        <v>3.243644532</v>
+        <v>0.202187044</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B27" t="n">
-        <v>1.438782402</v>
+        <v>2.141113051</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="B28" t="n">
-        <v>14.38747837</v>
+        <v>1.577063883</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B29" t="n">
-        <v>1.89660106</v>
+        <v>0.030829113</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B30" t="n">
-        <v>1.86650182</v>
+        <v>1.408626008</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B31" t="n">
-        <v>0.546306064</v>
+        <v>7.81758972</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B32" t="n">
-        <v>3.125688367</v>
+        <v>3.520069099</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="B33" t="n">
-        <v>1.625933957</v>
+        <v>2.419111192</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B34" t="n">
-        <v>2.675016686</v>
+        <v>1.883406477</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="B35" t="n">
-        <v>1.63010458</v>
+        <v>0.563753712</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="B36" t="n">
-        <v>1.163413673</v>
+        <v>1.229870838</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37"/>
+        <v>44</v>
+      </c>
+      <c r="B37" t="n">
+        <v>3.382151699</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B38" t="n">
-        <v>1.182252391</v>
+        <v>4.334403287</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B39" t="n">
-        <v>6.527998504</v>
+        <v>2.603885364</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40"/>
+        <v>47</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.065721209</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B41" t="n">
-        <v>0.823012001</v>
+        <v>1.457515543</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B42" t="n">
-        <v>14.97864358</v>
+        <v>2.640463722</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="B43" t="n">
-        <v>1.555069352</v>
+        <v>2.869007744</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="B44" t="n">
-        <v>1.789579143</v>
+        <v>3.27979297</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B45" t="n">
-        <v>17.88763843</v>
+        <v>2.115468512</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B46" t="n">
-        <v>1.580202818</v>
+        <v>4.253905226</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B47" t="n">
-        <v>23.81550264</v>
+        <v>1.691753096</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>70</v>
-      </c>
-      <c r="B48"/>
+        <v>55</v>
+      </c>
+      <c r="B48" t="n">
+        <v>2.045734377</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>71</v>
-      </c>
-      <c r="B49" t="n">
-        <v>16.35479354</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B49"/>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B50" t="n">
-        <v>8.789180489</v>
+        <v>1.057583525</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>75</v>
-      </c>
-      <c r="B51" t="n">
-        <v>49.44722943</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B51"/>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>76</v>
-      </c>
-      <c r="B52" t="n">
-        <v>2.355256429</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B52"/>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>77</v>
-      </c>
-      <c r="B53" t="n">
-        <v>1.812884594</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B53"/>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B54" t="n">
-        <v>13.72285981</v>
+        <v>7.102184186</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B55" t="n">
-        <v>2.320414688</v>
+        <v>1.37779521</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B56" t="n">
-        <v>12.9731581</v>
+        <v>0.912889569</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B57" t="n">
-        <v>0.957801758</v>
+        <v>10.96631953</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="B58" t="n">
-        <v>8.242166581</v>
+        <v>9.938296818</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="B59" t="n">
-        <v>0.596423192</v>
+        <v>0.648424056</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="B60" t="n">
-        <v>3.011438326</v>
+        <v>3.073305866</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>92</v>
-      </c>
-      <c r="B61"/>
+        <v>66</v>
+      </c>
+      <c r="B61" t="n">
+        <v>3.985654224</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="B62" t="n">
-        <v>3.440094174</v>
+        <v>7.562331028</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>94</v>
-      </c>
-      <c r="B63"/>
+        <v>7</v>
+      </c>
+      <c r="B63" t="n">
+        <v>1.655348691</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>5</v>
-      </c>
-      <c r="B64" t="n">
-        <v>1.106719661</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B64"/>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="B65" t="n">
-        <v>1.883875474</v>
+        <v>2.950981474</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B66" t="n">
-        <v>4.388483053</v>
+        <v>1.527187805</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>97</v>
-      </c>
-      <c r="B67"/>
+        <v>71</v>
+      </c>
+      <c r="B67" t="n">
+        <v>10.51478403</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>98</v>
-      </c>
-      <c r="B68"/>
+        <v>72</v>
+      </c>
+      <c r="B68" t="n">
+        <v>3.938739681</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>9</v>
-      </c>
-      <c r="B69"/>
+        <v>73</v>
+      </c>
+      <c r="B69" t="n">
+        <v>9.943570708</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="B70" t="n">
-        <v>10.14051046</v>
+        <v>15.94206339</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="B71" t="n">
-        <v>0.882331804</v>
+        <v>1.474987818</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="B72" t="n">
-        <v>1.056106401</v>
+        <v>5.468586952</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="B73" t="n">
-        <v>4.949204454</v>
+        <v>4.085344994</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="B74" t="n">
-        <v>2.894125184</v>
+        <v>6.689520165</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="B75" t="n">
-        <v>4.07684759</v>
+        <v>4.555951877</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="B76" t="n">
-        <v>2.644795613</v>
+        <v>5.393048514</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="B77" t="n">
-        <v>5.558078944</v>
+        <v>3.032703878</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="B78" t="n">
-        <v>0.794105668</v>
+        <v>2.454301232</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="B79" t="n">
-        <v>5.124140376</v>
+        <v>1.997174495</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="B80" t="n">
-        <v>0.230206164</v>
+        <v>6.96792064</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="B81" t="n">
-        <v>3.415749762</v>
+        <v>0.11500782</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
+        <v>86</v>
+      </c>
+      <c r="B82" t="n">
+        <v>5.265889176</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>87</v>
+      </c>
+      <c r="B83" t="n">
+        <v>4.860103146</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>88</v>
+      </c>
+      <c r="B84"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>89</v>
+      </c>
+      <c r="B85" t="n">
+        <v>4.098517151</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>90</v>
+      </c>
+      <c r="B86" t="n">
+        <v>5.005857661</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87" t="n">
+        <v>2.690890239</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>92</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0.363249229</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.654599749</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90" t="n">
+        <v>1.359278289</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" t="n">
+        <v>1.600830967</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92" t="n">
+        <v>1.465678143</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" t="n">
+        <v>1.644487678</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>97</v>
+      </c>
+      <c r="B94" t="n">
+        <v>3.581977002</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>98</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0.824085556</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>9</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0.240180388</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>99</v>
+      </c>
+      <c r="B97" t="n">
+        <v>1.687900821</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>101</v>
+      </c>
+      <c r="B99" t="n">
+        <v>2.620469746</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100" t="n">
+        <v>3.336437983</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" t="n">
+        <v>5.02134159</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>104</v>
+      </c>
+      <c r="B102" t="n">
+        <v>1.998034567</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>105</v>
+      </c>
+      <c r="B103" t="n">
+        <v>4.179304355</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>106</v>
+      </c>
+      <c r="B104" t="n">
+        <v>0.248657145</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>107</v>
+      </c>
+      <c r="B105" t="n">
+        <v>4.660560717</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>108</v>
+      </c>
+      <c r="B106" t="n">
+        <v>1.313051236</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>109</v>
+      </c>
+      <c r="B107" t="n">
+        <v>1.411956431</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>110</v>
+      </c>
+      <c r="B108" t="n">
+        <v>6.805162763</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>111</v>
+      </c>
+      <c r="B109" t="n">
+        <v>0.483606672</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" t="n">
+        <v>7.479174133</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" t="n">
+        <v>1.508198871</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
         <v>114</v>
       </c>
-      <c r="B82" t="n">
-        <v>1.157516618</v>
+      <c r="B112" t="n">
+        <v>0.883457294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>